<commit_message>
Added education, additional basic, location forms and linked to basic
</commit_message>
<xml_diff>
--- a/project/static/LifePartnerCriteria.xlsx
+++ b/project/static/LifePartnerCriteria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rk185212\Google Drive\Learning\Git\flask\Recommendation\match-life-partner\project\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BAFF14-5AB0-4A2B-8F62-6B1F026E1E16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48EA9D95-3486-46F3-8BD9-9895312AF1C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7632" tabRatio="297" xr2:uid="{CF5D7121-CE8E-4DE7-AD49-3A98B7171CA6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7632" tabRatio="393" firstSheet="1" activeTab="4" xr2:uid="{CF5D7121-CE8E-4DE7-AD49-3A98B7171CA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Person" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Vehicles" sheetId="6" r:id="rId4"/>
     <sheet name="Education" sheetId="4" r:id="rId5"/>
     <sheet name="Family" sheetId="2" r:id="rId6"/>
+    <sheet name="Location" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="113">
   <si>
     <t>Age</t>
   </si>
@@ -49,9 +50,6 @@
     <t>Height</t>
   </si>
   <si>
-    <t>Education</t>
-  </si>
-  <si>
     <t>Organization</t>
   </si>
   <si>
@@ -355,7 +353,28 @@
     <t>Dark</t>
   </si>
   <si>
-    <t>Hairs</t>
+    <t>HairKind</t>
+  </si>
+  <si>
+    <t>Thick</t>
+  </si>
+  <si>
+    <t>Sparse</t>
+  </si>
+  <si>
+    <t>BaldHead</t>
+  </si>
+  <si>
+    <t>Hobbies</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>PostalCode</t>
   </si>
 </sst>
 </file>
@@ -707,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18483076-4292-4E5D-A67B-6A3AF54A24CD}">
-  <dimension ref="A2:L4"/>
+  <dimension ref="A2:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -719,70 +738,77 @@
     <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H2" t="s">
-        <v>3</v>
+        <v>99</v>
       </c>
       <c r="I2" t="s">
-        <v>4</v>
+        <v>109</v>
       </c>
       <c r="J2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="K2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J3" t="s">
         <v>103</v>
       </c>
-      <c r="L2" t="s">
+      <c r="K3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="K3" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J4" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="K4" t="s">
-        <v>105</v>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K5" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -819,75 +845,75 @@
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
         <v>39</v>
       </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
       <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>9</v>
       </c>
-      <c r="K2" t="s">
-        <v>10</v>
-      </c>
       <c r="L2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N2" t="s">
         <v>101</v>
-      </c>
-      <c r="N2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -924,74 +950,74 @@
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I2" t="s">
+        <v>98</v>
+      </c>
+      <c r="J2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K2" t="s">
         <v>80</v>
       </c>
-      <c r="C2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F2" t="s">
-        <v>90</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="L2" t="s">
+        <v>83</v>
+      </c>
+      <c r="M2" t="s">
         <v>91</v>
       </c>
-      <c r="H2" t="s">
-        <v>83</v>
-      </c>
-      <c r="I2" t="s">
-        <v>99</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="N2" t="s">
+        <v>81</v>
+      </c>
+      <c r="O2" t="s">
         <v>97</v>
-      </c>
-      <c r="K2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L2" t="s">
-        <v>84</v>
-      </c>
-      <c r="M2" t="s">
-        <v>92</v>
-      </c>
-      <c r="N2" t="s">
-        <v>82</v>
-      </c>
-      <c r="O2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="L3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="L4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="L5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="L6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="L7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1017,31 +1043,31 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1054,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDE14EE5-F20E-4209-9974-ADF5F78D71E0}">
   <dimension ref="A2:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1072,134 +1098,134 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" t="s">
         <v>48</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>49</v>
       </c>
-      <c r="G2" t="s">
-        <v>50</v>
-      </c>
       <c r="H2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1212,7 +1238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C26EB87A-5C60-4C7B-807C-526B716A77BB}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
@@ -1246,75 +1272,75 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" t="s">
-        <v>20</v>
-      </c>
       <c r="M1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N1" t="s">
         <v>72</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>73</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>74</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>75</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>76</v>
-      </c>
-      <c r="R1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="E2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="E3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="E4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
@@ -1324,6 +1350,42 @@
       </c>
       <c r="G6" t="s">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19CB66EB-1EC0-45BC-B02F-9862D7CF3E39}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added family, education, profession, property and updated excel
</commit_message>
<xml_diff>
--- a/project/static/LifePartnerCriteria.xlsx
+++ b/project/static/LifePartnerCriteria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rk185212\Google Drive\Learning\Git\flask\Recommendation\match-life-partner\project\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48EA9D95-3486-46F3-8BD9-9895312AF1C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE99CCE1-D0A5-4787-9B0A-3CE35E71E9CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7632" tabRatio="393" firstSheet="1" activeTab="4" xr2:uid="{CF5D7121-CE8E-4DE7-AD49-3A98B7171CA6}"/>
   </bookViews>
@@ -56,9 +56,6 @@
     <t>Experience</t>
   </si>
   <si>
-    <t>HomeTown</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
@@ -152,15 +149,9 @@
     <t>Father</t>
   </si>
   <si>
-    <t>Profession</t>
-  </si>
-  <si>
     <t>ProfessionType</t>
   </si>
   <si>
-    <t>HighestEducation</t>
-  </si>
-  <si>
     <t>PartTime</t>
   </si>
   <si>
@@ -182,9 +173,6 @@
     <t>PursueStudyAfterMarriage</t>
   </si>
   <si>
-    <t>StudyFuturePlan</t>
-  </si>
-  <si>
     <t>StudyAbroad</t>
   </si>
   <si>
@@ -263,15 +251,6 @@
     <t>UnMarriedSisters</t>
   </si>
   <si>
-    <t>BrothersEmployed</t>
-  </si>
-  <si>
-    <t>SistersEmployed</t>
-  </si>
-  <si>
-    <t>Migrated</t>
-  </si>
-  <si>
     <t>Lands</t>
   </si>
   <si>
@@ -329,9 +308,6 @@
     <t>PropertyLoans</t>
   </si>
   <si>
-    <t>SettledProperty</t>
-  </si>
-  <si>
     <t>RentPaid</t>
   </si>
   <si>
@@ -375,6 +351,30 @@
   </si>
   <si>
     <t>PostalCode</t>
+  </si>
+  <si>
+    <t>Designation</t>
+  </si>
+  <si>
+    <t>MigratedFromHomeTown</t>
+  </si>
+  <si>
+    <t>FatherOccupation</t>
+  </si>
+  <si>
+    <t>MotherOccupation</t>
+  </si>
+  <si>
+    <t>BrothersOccupation</t>
+  </si>
+  <si>
+    <t>SistersOccupation</t>
+  </si>
+  <si>
+    <t>HighestQualification</t>
+  </si>
+  <si>
+    <t>DroppedEducation</t>
   </si>
 </sst>
 </file>
@@ -757,19 +757,19 @@
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -778,37 +778,37 @@
         <v>3</v>
       </c>
       <c r="H2" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="I2" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="J2" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="K2" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="J3" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="K3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="J4" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="K4" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K5" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -819,51 +819,54 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9913CE64-4E00-4397-9366-0A211BB0F805}">
-  <dimension ref="A2:N6"/>
+  <dimension ref="A2:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2" t="s">
         <v>6</v>
@@ -875,45 +878,54 @@
         <v>8</v>
       </c>
       <c r="K2" t="s">
-        <v>9</v>
+        <v>106</v>
       </c>
       <c r="L2" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="M2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="N2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+      <c r="O2" t="s">
+        <v>108</v>
+      </c>
+      <c r="P2" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" t="s">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" t="s">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="E6" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -924,14 +936,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D123F256-9F5A-4BE4-8134-C1A3CD225B75}">
-  <dimension ref="A2:O7"/>
+  <dimension ref="A2:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.88671875" bestFit="1" customWidth="1"/>
@@ -948,76 +961,73 @@
     <col min="15" max="15" width="13.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K2" t="s">
+        <v>73</v>
+      </c>
+      <c r="L2" t="s">
+        <v>76</v>
+      </c>
+      <c r="M2" t="s">
+        <v>84</v>
+      </c>
+      <c r="N2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L4" t="s">
         <v>35</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L7" t="s">
         <v>79</v>
-      </c>
-      <c r="C2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H2" t="s">
-        <v>82</v>
-      </c>
-      <c r="I2" t="s">
-        <v>98</v>
-      </c>
-      <c r="J2" t="s">
-        <v>96</v>
-      </c>
-      <c r="K2" t="s">
-        <v>80</v>
-      </c>
-      <c r="L2" t="s">
-        <v>83</v>
-      </c>
-      <c r="M2" t="s">
-        <v>91</v>
-      </c>
-      <c r="N2" t="s">
-        <v>81</v>
-      </c>
-      <c r="O2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="L3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="L4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="L5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="L6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="L7" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1043,31 +1053,31 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="E2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1081,7 +1091,7 @@
   <dimension ref="A2:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B22"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1091,141 +1101,141 @@
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" t="s">
         <v>40</v>
       </c>
-      <c r="C2" t="s">
-        <v>43</v>
-      </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>112</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1236,10 +1246,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C26EB87A-5C60-4C7B-807C-526B716A77BB}">
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+      <selection activeCell="Q1" sqref="Q1:R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1264,7 +1274,7 @@
     <col min="18" max="18" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1272,75 +1282,69 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" t="s">
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
         <v>20</v>
       </c>
-      <c r="F1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" t="s">
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
         <v>28</v>
-      </c>
-      <c r="K1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" t="s">
-        <v>71</v>
-      </c>
-      <c r="N1" t="s">
-        <v>72</v>
-      </c>
-      <c r="O1" t="s">
-        <v>73</v>
-      </c>
-      <c r="P1" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>75</v>
-      </c>
-      <c r="R1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
@@ -1363,29 +1367,29 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="E1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>